<commit_message>
Jo was in een goeie bui. Jurriën snapte zijn uitleg.
</commit_message>
<xml_diff>
--- a/DOE/opdrachten.xlsx
+++ b/DOE/opdrachten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="13.47" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,8 @@
     <sheet name="13.49" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="13.51" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="13.66" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="13.57" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="13.58" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
   <si>
     <t xml:space="preserve">nozzle type</t>
   </si>
@@ -163,6 +165,90 @@
   </si>
   <si>
     <t xml:space="preserve">82.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Temperatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.77</t>
   </si>
 </sst>
 </file>
@@ -256,7 +342,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -283,6 +369,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -430,7 +520,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,7 +705,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="9.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,7 +1269,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1268,6 +1358,282 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>1245</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>1235</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>1285</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>1245</v>
+      </c>
+      <c r="F3" s="6" t="n">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>1235</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>1240</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>1220</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>1225</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>1170</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>1155</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>